<commit_message>
Rf file with gamma
</commit_message>
<xml_diff>
--- a/Rf.xlsx
+++ b/Rf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchicagoedu-my.sharepoint.com/personal/rishaq_uchicago_edu/Documents/Desktop/2. RA-SHIP/SUMMER PROJECTS/ACLI/For BI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uchicagoedu-my.sharepoint.com/personal/rishaq_uchicago_edu/Documents/Desktop/2. RA-SHIP/SUMMER PROJECTS/ACLI/Python/dash-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048F7511A67645ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C525E6F-E0F8-4E5E-8BAB-5580BB06A2FE}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048F7511A67645ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D0E5CE8-218E-4767-8AC4-A18E65E33C46}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Quarter</t>
   </si>
   <si>
     <t>Rf</t>
+  </si>
+  <si>
+    <t>Structural Differences</t>
   </si>
 </sst>
 </file>
@@ -373,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C119"/>
+  <dimension ref="B2:D119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -383,950 +386,1305 @@
   <cols>
     <col min="1" max="1" width="1.36328125" customWidth="1"/>
     <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="2">
         <v>35155</v>
       </c>
       <c r="C3" s="3">
         <v>5.79E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D3" s="3">
+        <v>6.0900000000000003E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>35246</v>
       </c>
       <c r="C4" s="3">
         <v>6.6566666666666677E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D4" s="3">
+        <v>6.9566666666666679E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>35338</v>
       </c>
       <c r="C5" s="3">
         <v>6.6699999999999995E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D5" s="3">
+        <v>6.9699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>35430</v>
       </c>
       <c r="C6" s="3">
         <v>6.239999999999999E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D6" s="3">
+        <v>6.5399999999999986E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <v>35520</v>
       </c>
       <c r="C7" s="3">
         <v>6.480000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D7" s="3">
+        <v>6.7800000000000013E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>35611</v>
       </c>
       <c r="C8" s="3">
         <v>6.6600000000000006E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D8" s="3">
+        <v>6.9600000000000009E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>35703</v>
       </c>
       <c r="C9" s="3">
         <v>6.2300000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D9" s="3">
+        <v>6.5299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>35795</v>
       </c>
       <c r="C10" s="3">
         <v>5.9266666666666662E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D10" s="3">
+        <v>6.2266666666666665E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>35885</v>
       </c>
       <c r="C11" s="3">
         <v>5.6133333333333334E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D11" s="3">
+        <v>5.9133333333333329E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>35976</v>
       </c>
       <c r="C12" s="3">
         <v>5.6600000000000004E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D12" s="3">
+        <v>5.9600000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>36068</v>
       </c>
       <c r="C13" s="3">
         <v>5.2133333333333337E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D13" s="3">
+        <v>5.513333333333334E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <v>36160</v>
       </c>
       <c r="C14" s="3">
         <v>4.6300000000000008E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D14" s="3">
+        <v>4.9300000000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="2">
         <v>36250</v>
       </c>
       <c r="C15" s="3">
         <v>5.0866666666666671E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D15" s="3">
+        <v>5.3866666666666667E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>36341</v>
       </c>
       <c r="C16" s="3">
         <v>5.6566666666666661E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="3">
+        <v>5.9566666666666664E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>36433</v>
       </c>
       <c r="C17" s="3">
         <v>6.0700000000000004E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="3">
+        <v>6.3700000000000007E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>36525</v>
       </c>
       <c r="C18" s="3">
         <v>6.2933333333333327E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="3">
+        <v>6.593333333333333E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>36616</v>
       </c>
       <c r="C19" s="3">
         <v>6.643333333333333E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="3">
+        <v>6.9433333333333333E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>36707</v>
       </c>
       <c r="C20" s="3">
         <v>6.4299999999999996E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="3">
+        <v>6.7299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>36799</v>
       </c>
       <c r="C21" s="3">
         <v>6.083333333333333E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D21" s="3">
+        <v>6.3833333333333325E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>36891</v>
       </c>
       <c r="C22" s="3">
         <v>5.6333333333333326E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="3">
+        <v>5.9333333333333321E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>36981</v>
       </c>
       <c r="C23" s="3">
         <v>5.0366666666666671E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D23" s="3">
+        <v>5.3366666666666673E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>37072</v>
       </c>
       <c r="C24" s="3">
         <v>5.1366666666666672E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D24" s="3">
+        <v>5.4366666666666667E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="2">
         <v>37164</v>
       </c>
       <c r="C25" s="3">
         <v>4.8033333333333338E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D25" s="3">
+        <v>5.103333333333334E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="2">
         <v>37256</v>
       </c>
       <c r="C26" s="3">
         <v>4.53E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="3">
+        <v>4.8299999999999996E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="2">
         <v>37346</v>
       </c>
       <c r="C27" s="3">
         <v>4.8800000000000003E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="3">
+        <v>5.1800000000000006E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="2">
         <v>37437</v>
       </c>
       <c r="C28" s="3">
         <v>4.8399999999999999E-2</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="3">
+        <v>5.1400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="2">
         <v>37529</v>
       </c>
       <c r="C29" s="3">
         <v>3.8933333333333334E-2</v>
       </c>
-    </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D29" s="3">
+        <v>4.1933333333333336E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="2">
         <v>37621</v>
       </c>
       <c r="C30" s="3">
         <v>3.6033333333333334E-2</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D30" s="3">
+        <v>3.903333333333333E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="2">
         <v>37711</v>
       </c>
       <c r="C31" s="3">
         <v>3.4633333333333335E-2</v>
       </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D31" s="3">
+        <v>3.7633333333333331E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="2">
         <v>37802</v>
       </c>
       <c r="C32" s="3">
         <v>3.1266666666666665E-2</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D32" s="3">
+        <v>3.4266666666666667E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="2">
         <v>37894</v>
       </c>
       <c r="C33" s="3">
         <v>3.7166666666666667E-2</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D33" s="3">
+        <v>4.016666666666667E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="2">
         <v>37986</v>
       </c>
       <c r="C34" s="3">
         <v>3.7833333333333337E-2</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D34" s="3">
+        <v>4.083333333333334E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="2">
         <v>38077</v>
       </c>
       <c r="C35" s="3">
         <v>3.5166666666666659E-2</v>
       </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D35" s="3">
+        <v>3.8166666666666661E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="2">
         <v>38168</v>
       </c>
       <c r="C36" s="3">
         <v>4.1833333333333333E-2</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D36" s="3">
+        <v>4.4833333333333329E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="2">
         <v>38260</v>
       </c>
       <c r="C37" s="3">
         <v>3.9200000000000006E-2</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D37" s="3">
+        <v>4.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="2">
         <v>38352</v>
       </c>
       <c r="C38" s="3">
         <v>3.8533333333333336E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D38" s="3">
+        <v>4.1533333333333339E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="2">
         <v>38442</v>
       </c>
       <c r="C39" s="3">
         <v>4.0899999999999999E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D39" s="3">
+        <v>4.3900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="2">
         <v>38533</v>
       </c>
       <c r="C40" s="3">
         <v>3.9866666666666661E-2</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="3">
+        <v>4.2866666666666657E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="2">
         <v>38625</v>
       </c>
       <c r="C41" s="3">
         <v>4.1066666666666668E-2</v>
       </c>
-    </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D41" s="3">
+        <v>4.4066666666666671E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" s="2">
         <v>38717</v>
       </c>
       <c r="C42" s="3">
         <v>4.423333333333334E-2</v>
       </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D42" s="3">
+        <v>4.7233333333333336E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="2">
         <v>38807</v>
       </c>
       <c r="C43" s="3">
         <v>4.5466666666666662E-2</v>
       </c>
-    </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D43" s="3">
+        <v>4.8466666666666658E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" s="2">
         <v>38898</v>
       </c>
       <c r="C44" s="3">
         <v>5.0166666666666672E-2</v>
       </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D44" s="3">
+        <v>5.3166666666666675E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" s="2">
         <v>38990</v>
       </c>
       <c r="C45" s="3">
         <v>4.8533333333333338E-2</v>
       </c>
-    </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D45" s="3">
+        <v>5.1533333333333341E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="2">
         <v>39082</v>
       </c>
       <c r="C46" s="3">
         <v>4.6033333333333336E-2</v>
       </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D46" s="3">
+        <v>4.9033333333333338E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="2">
         <v>39172</v>
       </c>
       <c r="C47" s="3">
         <v>4.6533333333333336E-2</v>
       </c>
-    </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D47" s="3">
+        <v>4.9533333333333339E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" s="2">
         <v>39263</v>
       </c>
       <c r="C48" s="3">
         <v>4.7866666666666668E-2</v>
       </c>
-    </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D48" s="3">
+        <v>5.0866666666666671E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" s="2">
         <v>39355</v>
       </c>
       <c r="C49" s="3">
         <v>4.5966666666666663E-2</v>
       </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D49" s="3">
+        <v>4.8966666666666665E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="2">
         <v>39447</v>
       </c>
       <c r="C50" s="3">
         <v>3.9799999999999995E-2</v>
       </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D50" s="3">
+        <v>4.2799999999999991E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="2">
         <v>39538</v>
       </c>
       <c r="C51" s="3">
         <v>3.15E-2</v>
       </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D51" s="3">
+        <v>3.4500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="2">
         <v>39629</v>
       </c>
       <c r="C52" s="3">
         <v>3.4599999999999999E-2</v>
       </c>
-    </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D52" s="3">
+        <v>3.7599999999999995E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" s="2">
         <v>39721</v>
       </c>
       <c r="C53" s="3">
         <v>3.4366666666666663E-2</v>
       </c>
-    </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D53" s="3">
+        <v>3.7366666666666673E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54" s="2">
         <v>39813</v>
       </c>
       <c r="C54" s="3">
         <v>2.6333333333333334E-2</v>
       </c>
-    </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D54" s="3">
+        <v>2.9333333333333326E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="2">
         <v>39903</v>
       </c>
       <c r="C55" s="3">
         <v>2.2333333333333334E-2</v>
       </c>
-    </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D55" s="3">
+        <v>2.5333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="2">
         <v>39994</v>
       </c>
       <c r="C56" s="3">
         <v>2.8833333333333332E-2</v>
       </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D56" s="3">
+        <v>3.1833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="2">
         <v>40086</v>
       </c>
       <c r="C57" s="3">
         <v>3.1233333333333335E-2</v>
       </c>
-    </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D57" s="3">
+        <v>3.4233333333333338E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="2">
         <v>40178</v>
       </c>
       <c r="C58" s="3">
         <v>2.9833333333333333E-2</v>
       </c>
-    </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D58" s="3">
+        <v>3.2833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="2">
         <v>40268</v>
       </c>
       <c r="C59" s="3">
         <v>3.1633333333333333E-2</v>
       </c>
-    </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D59" s="3">
+        <v>3.4633333333333335E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60" s="2">
         <v>40359</v>
       </c>
       <c r="C60" s="3">
         <v>2.9333333333333333E-2</v>
       </c>
-    </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D60" s="3">
+        <v>3.2333333333333332E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="2">
         <v>40451</v>
       </c>
       <c r="C61" s="3">
         <v>2.1933333333333332E-2</v>
       </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D61" s="3">
+        <v>2.4933333333333328E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="2">
         <v>40543</v>
       </c>
       <c r="C62" s="3">
         <v>2.1766666666666667E-2</v>
       </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D62" s="3">
+        <v>2.4766666666666666E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="2">
         <v>40633</v>
       </c>
       <c r="C63" s="3">
         <v>2.8266666666666666E-2</v>
       </c>
-    </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D63" s="3">
+        <v>3.1266666666666665E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64" s="2">
         <v>40724</v>
       </c>
       <c r="C64" s="3">
         <v>2.5466666666666665E-2</v>
       </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D64" s="3">
+        <v>2.8466666666666668E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B65" s="2">
         <v>40816</v>
       </c>
       <c r="C65" s="3">
         <v>1.7766666666666663E-2</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D65" s="3">
+        <v>2.0766666666666662E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B66" s="2">
         <v>40908</v>
       </c>
       <c r="C66" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D66" s="3">
+        <v>1.8000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B67" s="2">
         <v>40999</v>
       </c>
       <c r="C67" s="3">
         <v>1.4366666666666666E-2</v>
       </c>
-    </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D67" s="3">
+        <v>1.7366666666666662E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B68" s="2">
         <v>41090</v>
       </c>
       <c r="C68" s="3">
         <v>1.24E-2</v>
       </c>
-    </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D68" s="3">
+        <v>1.5399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="2">
         <v>41182</v>
       </c>
       <c r="C69" s="3">
         <v>1.0799999999999999E-2</v>
       </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D69" s="3">
+        <v>1.3800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B70" s="2">
         <v>41274</v>
       </c>
       <c r="C70" s="3">
         <v>1.12E-2</v>
       </c>
-    </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D70" s="3">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B71" s="2">
         <v>41364</v>
       </c>
       <c r="C71" s="3">
         <v>1.3233333333333333E-2</v>
       </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D71" s="3">
+        <v>1.6233333333333332E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="2">
         <v>41455</v>
       </c>
       <c r="C72" s="3">
         <v>1.3900000000000001E-2</v>
       </c>
-    </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D72" s="3">
+        <v>1.6899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="2">
         <v>41547</v>
       </c>
       <c r="C73" s="3">
         <v>2.12E-2</v>
       </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D73" s="3">
+        <v>2.4199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="2">
         <v>41639</v>
       </c>
       <c r="C74" s="3">
         <v>2.1166666666666667E-2</v>
       </c>
-    </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D74" s="3">
+        <v>2.416666666666667E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B75" s="2">
         <v>41729</v>
       </c>
       <c r="C75" s="3">
         <v>2.2233333333333331E-2</v>
       </c>
-    </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D75" s="3">
+        <v>2.5233333333333326E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="2">
         <v>41820</v>
       </c>
       <c r="C76" s="3">
         <v>2.1933333333333332E-2</v>
       </c>
-    </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D76" s="3">
+        <v>2.4933333333333332E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B77" s="2">
         <v>41912</v>
       </c>
       <c r="C77" s="3">
         <v>2.1566666666666665E-2</v>
       </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D77" s="3">
+        <v>2.4566666666666664E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="2">
         <v>42004</v>
       </c>
       <c r="C78" s="3">
         <v>1.9966666666666664E-2</v>
       </c>
-    </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D78" s="3">
+        <v>2.2966666666666663E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B79" s="2">
         <v>42094</v>
       </c>
       <c r="C79" s="3">
         <v>1.7666666666666667E-2</v>
       </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D79" s="3">
+        <v>2.0666666666666667E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B80" s="2">
         <v>42185</v>
       </c>
       <c r="C80" s="3">
         <v>1.9066666666666666E-2</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D80" s="3">
+        <v>2.2066666666666665E-2</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" s="2">
         <v>42277</v>
       </c>
       <c r="C81" s="3">
         <v>1.9433333333333334E-2</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D81" s="3">
+        <v>2.2433333333333333E-2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82" s="2">
         <v>42369</v>
       </c>
       <c r="C82" s="3">
         <v>1.9400000000000001E-2</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D82" s="3">
+        <v>2.2400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B83" s="2">
         <v>42460</v>
       </c>
       <c r="C83" s="3">
         <v>1.6866666666666669E-2</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D83" s="3">
+        <v>1.9866666666666668E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" s="2">
         <v>42551</v>
       </c>
       <c r="C84" s="3">
         <v>1.5366666666666667E-2</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D84" s="3">
+        <v>1.836666666666667E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" s="2">
         <v>42643</v>
       </c>
       <c r="C85" s="3">
         <v>1.3966666666666667E-2</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D85" s="3">
+        <v>1.6966666666666672E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B86" s="2">
         <v>42735</v>
       </c>
       <c r="C86" s="3">
         <v>1.9266666666666668E-2</v>
       </c>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D86" s="3">
+        <v>2.2266666666666667E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" s="2">
         <v>42825</v>
       </c>
       <c r="C87" s="3">
         <v>2.2500000000000003E-2</v>
       </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D87" s="3">
+        <v>2.5500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B88" s="2">
         <v>42916</v>
       </c>
       <c r="C88" s="3">
         <v>2.0733333333333329E-2</v>
       </c>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D88" s="3">
+        <v>2.3733333333333329E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B89" s="2">
         <v>43008</v>
       </c>
       <c r="C89" s="3">
         <v>2.0633333333333333E-2</v>
       </c>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D89" s="3">
+        <v>2.3633333333333333E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90" s="2">
         <v>43100</v>
       </c>
       <c r="C90" s="3">
         <v>2.2500000000000003E-2</v>
       </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D90" s="3">
+        <v>2.5500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B91" s="2">
         <v>43190</v>
       </c>
       <c r="C91" s="3">
         <v>2.6866666666666664E-2</v>
       </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D91" s="3">
+        <v>2.9866666666666663E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B92" s="2">
         <v>43281</v>
       </c>
       <c r="C92" s="3">
         <v>2.8733333333333333E-2</v>
       </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D92" s="3">
+        <v>3.1733333333333336E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B93" s="2">
         <v>43373</v>
       </c>
       <c r="C93" s="3">
         <v>2.8833333333333332E-2</v>
       </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D93" s="3">
+        <v>3.1833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B94" s="2">
         <v>43465</v>
       </c>
       <c r="C94" s="3">
         <v>2.9599999999999998E-2</v>
       </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D94" s="3">
+        <v>3.2599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B95" s="2">
         <v>43555</v>
       </c>
       <c r="C95" s="3">
         <v>2.5499999999999998E-2</v>
       </c>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D95" s="3">
+        <v>2.8499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B96" s="2">
         <v>43646</v>
       </c>
       <c r="C96" s="3">
         <v>2.2233333333333338E-2</v>
       </c>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D96" s="3">
+        <v>2.5233333333333333E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B97" s="2">
         <v>43738</v>
       </c>
       <c r="C97" s="3">
         <v>1.7066666666666664E-2</v>
       </c>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D97" s="3">
+        <v>2.0066666666666667E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B98" s="2">
         <v>43830</v>
       </c>
       <c r="C98" s="3">
         <v>1.7166666666666667E-2</v>
       </c>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D98" s="3">
+        <v>2.0166666666666666E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B99" s="2">
         <v>43921</v>
       </c>
       <c r="C99" s="3">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D99" s="3">
+        <v>1.5899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B100" s="2">
         <v>44012</v>
       </c>
       <c r="C100" s="3">
         <v>5.4333333333333343E-3</v>
       </c>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D100" s="3">
+        <v>8.4333333333333361E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B101" s="2">
         <v>44104</v>
       </c>
       <c r="C101" s="3">
         <v>4.5999999999999999E-3</v>
       </c>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D101" s="3">
+        <v>7.6E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B102" s="2">
         <v>44196</v>
       </c>
       <c r="C102" s="3">
         <v>6.1333333333333335E-3</v>
       </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D102" s="3">
+        <v>9.1333333333333318E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B103" s="2">
         <v>44286</v>
       </c>
       <c r="C103" s="3">
         <v>9.8333333333333345E-3</v>
       </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D103" s="3">
+        <v>1.2833333333333335E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B104" s="2">
         <v>44377</v>
       </c>
       <c r="C104" s="3">
         <v>1.2733333333333333E-2</v>
       </c>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D104" s="3">
+        <v>1.5733333333333332E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B105" s="2">
         <v>44469</v>
       </c>
       <c r="C105" s="3">
         <v>1.0966666666666666E-2</v>
       </c>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D105" s="3">
+        <v>1.3966666666666665E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B106" s="2">
         <v>44561</v>
       </c>
       <c r="C106" s="3">
         <v>1.4166666666666666E-2</v>
       </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D106" s="3">
+        <v>1.7166666666666667E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B107" s="2">
         <v>44651</v>
       </c>
       <c r="C107" s="3">
         <v>1.9199999999999998E-2</v>
       </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D107" s="3">
+        <v>2.2199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B108" s="2">
         <v>44742</v>
       </c>
       <c r="C108" s="3">
         <v>2.9766666666666663E-2</v>
       </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D108" s="3">
+        <v>3.2766666666666666E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B109" s="2">
         <v>44834</v>
       </c>
       <c r="C109" s="3">
         <v>3.1966666666666664E-2</v>
       </c>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D109" s="3">
+        <v>3.4966666666666667E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B110" s="2">
         <v>44926</v>
       </c>
       <c r="C110" s="3">
         <v>3.9333333333333338E-2</v>
       </c>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D110" s="3">
+        <v>4.2333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B111" s="2">
         <v>45016</v>
       </c>
       <c r="C111" s="3">
         <v>3.7399999999999996E-2</v>
       </c>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D111" s="3">
+        <v>4.0399999999999998E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B112" s="2">
         <v>45107</v>
       </c>
       <c r="C112" s="3">
         <v>3.6433333333333338E-2</v>
       </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D112" s="3">
+        <v>3.9433333333333341E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B113" s="2">
         <v>45199</v>
       </c>
       <c r="C113" s="3">
         <v>4.2500000000000003E-2</v>
       </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D113" s="3">
+        <v>4.5499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114" s="2">
         <v>45291</v>
       </c>
       <c r="C114" s="3">
         <v>4.463333333333333E-2</v>
       </c>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D114" s="3">
+        <v>4.7633333333333326E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B115" s="2">
         <v>45382</v>
       </c>
       <c r="C115" s="3">
         <v>4.1500000000000002E-2</v>
       </c>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D115" s="3">
+        <v>4.4500000000000005E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B116" s="2">
         <v>45473</v>
       </c>
       <c r="C116" s="3">
         <v>4.4500000000000005E-2</v>
       </c>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D116" s="3">
+        <v>4.7500000000000007E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B117" s="2">
         <v>45565</v>
       </c>
       <c r="C117" s="3">
         <v>3.8533333333333336E-2</v>
       </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D117" s="3">
+        <v>4.1533333333333339E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B118" s="2">
         <v>45657</v>
       </c>
       <c r="C118" s="3">
         <v>4.2000000000000003E-2</v>
       </c>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="D118" s="3">
+        <v>4.5000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B119" s="2">
         <v>45747</v>
       </c>
       <c r="C119" s="3">
         <v>4.3533333333333334E-2</v>
+      </c>
+      <c r="D119" s="3">
+        <v>4.6533333333333336E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>